<commit_message>
4/7 minor transition bugs
</commit_message>
<xml_diff>
--- a/12.xlsx
+++ b/12.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Comp 380" r:id="rId3" sheetId="1"/>
+    <sheet name="2" r:id="rId3" sheetId="1"/>
     <sheet name="Comp 420" r:id="rId4" sheetId="2"/>
     <sheet name="test" r:id="rId5" sheetId="3"/>
     <sheet name="fasf" r:id="rId6" sheetId="4"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>140</t>
+  </si>
+  <si>
+    <t>42424</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -151,19 +160,19 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4/10 Added styling to alert boxes and fixed icon image uploads
</commit_message>
<xml_diff>
--- a/12.xlsx
+++ b/12.xlsx
@@ -6,17 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2" r:id="rId3" sheetId="1"/>
-    <sheet name="Comp 420" r:id="rId4" sheetId="2"/>
-    <sheet name="test" r:id="rId5" sheetId="3"/>
-    <sheet name="fasf" r:id="rId6" sheetId="4"/>
-    <sheet name="12" r:id="rId7" sheetId="5"/>
+    <sheet name="Geo 121" r:id="rId4" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="35">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -116,6 +112,12 @@
   <si>
     <t>136</t>
   </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
 </sst>
 </file>
 
@@ -157,105 +159,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -269,52 +172,19 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4/12 Added hover effects to buttons and general UI Polish
</commit_message>
<xml_diff>
--- a/12.xlsx
+++ b/12.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -118,6 +118,9 @@
   <si>
     <t>179</t>
   </si>
+  <si>
+    <t>242</t>
+  </si>
 </sst>
 </file>
 
@@ -178,13 +181,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4/19 Add assignemnt and student work. Just some clutter from trying to get table working
</commit_message>
<xml_diff>
--- a/12.xlsx
+++ b/12.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>242</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>01/05/1235</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>01/10/1001</t>
+  </si>
+  <si>
+    <t>Fisrt</t>
+  </si>
+  <si>
+    <t>Last</t>
   </si>
 </sst>
 </file>
@@ -190,6 +211,40 @@
         <v>35</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>